<commit_message>
AN170 test cycle 4 updated scripts
</commit_message>
<xml_diff>
--- a/src/Pickles/MIL_pickles/Output/AN170/AN170_TestScript_Desktop_Admin_System_FR_NFR.xlsx
+++ b/src/Pickles/MIL_pickles/Output/AN170/AN170_TestScript_Desktop_Admin_System_FR_NFR.xlsx
@@ -11,8 +11,10 @@
     <x:sheet name="CUSTOMERWORKFLOWUK" sheetId="4" r:id="rId4"/>
     <x:sheet name="DESKTOPLICENSING" sheetId="5" r:id="rId5"/>
     <x:sheet name="FOLDERWATCHER" sheetId="6" r:id="rId6"/>
-    <x:sheet name="UPDATECLIENT" sheetId="7" r:id="rId7"/>
-    <x:sheet name="USERDATA" sheetId="8" r:id="rId8"/>
+    <x:sheet name="OPENIMAGE" sheetId="7" r:id="rId7"/>
+    <x:sheet name="SHELLINTEGRATION" sheetId="8" r:id="rId8"/>
+    <x:sheet name="UPDATECLIENT" sheetId="9" r:id="rId9"/>
+    <x:sheet name="USERDATA" sheetId="10" r:id="rId10"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -20,9 +22,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
-  <x:si>
-    <x:t>CUstomerWorkflowEU</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="205">
+  <x:si>
+    <x:t>CustomerWorkflowEU</x:t>
   </x:si>
   <x:si>
     <x:t>Tags:</x:t>
@@ -49,93 +51,93 @@
     <x:t>I start Assistdent</x:t>
   </x:si>
   <x:si>
+    <x:t>the user registration form is displayed</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">When </x:t>
+  </x:si>
+  <x:si>
+    <x:t>I enter valid details</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I select "Germany" for the country</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Then </x:t>
+  </x:si>
+  <x:si>
+    <x:t>the registration is successful</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AssistDent starts</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TakePaymentEU:</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR031-2, @UR029-2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I have register a trial licence for an EU user</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I access the purchase licence page</x:t>
+  </x:si>
+  <x:si>
+    <x:t>choose the default price</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the payment is in Euros</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UK VAT is not applied</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ViewInvoiceEuro:</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR031-3, @UR029-3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I have paid for a subscription for an EU user</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I access my billing portal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I can view an invoice for each month</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the invoice contains the price paid</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the invoice contains the customer name and address</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the invoice contains a statement regarding reverse tax</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CustomerWorkflowUK</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR, @FR030, @UR028, @Admin, @DesktopOnly</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ShowRegistrationForm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR030-1, @UR028-1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CanRegisterInUK</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR030-2, @UR028-1</x:t>
+  </x:si>
+  <x:si>
     <x:t>the use registration form is displayed</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">When </x:t>
-  </x:si>
-  <x:si>
-    <x:t>I enter valid details</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I select "Germany" for the country</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Then </x:t>
-  </x:si>
-  <x:si>
-    <x:t>the registration is successful</x:t>
-  </x:si>
-  <x:si>
-    <x:t>AssistDent starts</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TakePaymentEU:</x:t>
-  </x:si>
-  <x:si>
-    <x:t>@FR031-2, @UR029-2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I have register a trial licence for an EU user</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I access the purchase licence page</x:t>
-  </x:si>
-  <x:si>
-    <x:t>choose the default price</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the payment is in Euros</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UK VAT is not applied</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ViewInvoiceEuro:</x:t>
-  </x:si>
-  <x:si>
-    <x:t>@FR031-3, @UR029-3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I have paid for a subscription for an EU user</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I access my billing portal</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I can view an invoice for each month</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the invoice contains the price paid</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the invoice contains the customer name and address</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the invoice contains a statement regarding reverse tax</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CustomerWorkflowUK</x:t>
-  </x:si>
-  <x:si>
-    <x:t>@FR, @FR030, @UR028, @Admin, @DesktopOnly</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ShowRegistrationForm</x:t>
-  </x:si>
-  <x:si>
-    <x:t>@FR030-1, @UR028-1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>the user registration form is displayed</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CanRegisterInUK</x:t>
-  </x:si>
-  <x:si>
-    <x:t>@FR030-2, @UR028-1</x:t>
-  </x:si>
-  <x:si>
     <x:t>I select "United Kingdom" for the country</x:t>
   </x:si>
   <x:si>
@@ -434,6 +436,129 @@
   </x:si>
   <x:si>
     <x:t>an informative message is displayed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OpenImage</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR, @FR036, @UR034, @Admin, @DesktopOnly</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR035-01, @UR034-01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I have started AssistDent from the desktop shortcut</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I select an image</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the selected image opens in AssistDent</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR035-01, @UR034-02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I have started AssistDent from the start menu</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DontOpenNonImage</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR035-02, @UR034-03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I select a text file</x:t>
+  </x:si>
+  <x:si>
+    <x:t>an error message is displayed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CancelOpenImage</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR035-03, @UR034-03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I have analysed an image in AssistDent</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I click the Browse Image button</x:t>
+  </x:si>
+  <x:si>
+    <x:t>click cancel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the previous image is still active</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OpenSecondImage</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR035-04, @UR034-03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I click the Open Image button</x:t>
+  </x:si>
+  <x:si>
+    <x:t>select an image</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ShellIntegration</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR, @FR035, @UR033, @Admin, @DesktopOnly</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OpenWith</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR035-01, @UR033-01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I have an image file</x:t>
+  </x:si>
+  <x:si>
+    <x:t>in Explorer I right click choose open with and find AssistDent.exe</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the image opens in AssistDent</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR035-02, @UR033-01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I have a text file</x:t>
+  </x:si>
+  <x:si>
+    <x:t>nothing happens</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DontOpenMultipleImages</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR035-03, @UR033-01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I have multiple image files</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR035-04, @UR033-02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>in Explorer I right click choose Open With AssistDent</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR035-05, @UR033-02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>in Explorer I right click</x:t>
+  </x:si>
+  <x:si>
+    <x:t>the Open With AssistDent menu option is not visible</x:t>
+  </x:si>
+  <x:si>
+    <x:t>@FR035-06, @UR033-02</x:t>
   </x:si>
   <x:si>
     <x:t>UpdateClient</x:t>
@@ -960,7 +1085,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B8"/>
+  <x:dimension ref="A1:B10"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -968,7 +1093,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:2">
       <x:c r="A1" s="1" t="s">
-        <x:v>162</x:v>
+        <x:v>203</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:2">
@@ -997,23 +1122,35 @@
       </x:c>
     </x:row>
     <x:row r="7" spans="1:2">
-      <x:c r="A7" s="1" t="s">
-        <x:v>163</x:v>
+      <x:c r="B7" s="6" t="s">
+        <x:v>160</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:2">
       <x:c r="B8" s="6" t="s">
-        <x:v>151</x:v>
+        <x:v>179</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:2">
+      <x:c r="A9" s="1" t="s">
+        <x:v>204</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:2">
+      <x:c r="B10" s="6" t="s">
+        <x:v>192</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="B2" location="'CUSTOMERWORKFLOWEU'!A1" display="CUstomerWorkflowEU"/>
+    <x:hyperlink ref="B2" location="'CUSTOMERWORKFLOWEU'!A1" display="CustomerWorkflowEU"/>
     <x:hyperlink ref="B3" location="'CUSTOMERWORKFLOWUK'!A1" display="CustomerWorkflowUK"/>
     <x:hyperlink ref="B4" location="'DESKTOPLICENSING'!A1" display="DesktopLicensing"/>
     <x:hyperlink ref="B5" location="'FOLDERWATCHER'!A1" display="FolderWatcher"/>
-    <x:hyperlink ref="B6" location="'UPDATECLIENT'!A1" display="UpdateClient"/>
-    <x:hyperlink ref="B8" location="'USERDATA'!A1" display="UserData"/>
+    <x:hyperlink ref="B6" location="'OPENIMAGE'!A1" display="OpenImage"/>
+    <x:hyperlink ref="B7" location="'SHELLINTEGRATION'!A1" display="ShellIntegration"/>
+    <x:hyperlink ref="B8" location="'UPDATECLIENT'!A1" display="UpdateClient"/>
+    <x:hyperlink ref="B10" location="'USERDATA'!A1" display="UserData"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1303,12 +1440,12 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
       <x:c r="B12" s="1" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
@@ -1316,7 +1453,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C13" s="2" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4"/>
@@ -1341,7 +1478,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:4">
@@ -1623,7 +1760,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:5">
@@ -1693,7 +1830,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:5">
@@ -2568,7 +2705,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D20"/>
+  <x:dimension ref="A1:D40"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -2590,7 +2727,7 @@
     <x:row r="3" spans="1:4"/>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>140</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -2598,7 +2735,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>141</x:v>
+        <x:v>140</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -2607,7 +2744,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>142</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
@@ -2615,7 +2752,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>142</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
@@ -2623,12 +2760,12 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>143</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
       <x:c r="B12" s="1" t="s">
-        <x:v>145</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
@@ -2636,7 +2773,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C13" s="2" t="s">
-        <x:v>146</x:v>
+        <x:v>144</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4"/>
@@ -2645,7 +2782,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>145</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:4">
@@ -2653,7 +2790,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>142</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4">
@@ -2661,31 +2798,137 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>144</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:4">
-      <x:c r="C18" s="3" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D18" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:4">
+      <x:c r="B19" s="1" t="s">
+        <x:v>146</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:4">
+      <x:c r="B20" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C20" s="2" t="s">
+        <x:v>147</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:4"/>
+    <x:row r="22" spans="1:4">
+      <x:c r="C22" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>141</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:4">
+      <x:c r="C23" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
         <x:v>148</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:4">
-      <x:c r="C19" s="3" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D19" s="0" t="s">
+    <x:row r="24" spans="1:4">
+      <x:c r="C24" s="3" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
         <x:v>149</x:v>
       </x:c>
     </x:row>
-    <x:row r="20" spans="1:4">
-      <x:c r="C20" s="3" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D20" s="0" t="s">
+    <x:row r="26" spans="1:4">
+      <x:c r="B26" s="1" t="s">
         <x:v>150</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:4">
+      <x:c r="B27" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C27" s="2" t="s">
+        <x:v>151</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:4"/>
+    <x:row r="29" spans="1:4">
+      <x:c r="C29" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:4">
+      <x:c r="C30" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>153</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:4">
+      <x:c r="C31" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>154</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:4">
+      <x:c r="C32" s="3" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>155</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:4">
+      <x:c r="B34" s="1" t="s">
+        <x:v>156</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:4">
+      <x:c r="B35" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C35" s="2" t="s">
+        <x:v>157</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:4"/>
+    <x:row r="37" spans="1:4">
+      <x:c r="C37" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D37" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:4">
+      <x:c r="C38" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:4">
+      <x:c r="C39" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D39" s="0" t="s">
+        <x:v>159</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:4">
+      <x:c r="C40" s="3" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D40" s="0" t="s">
+        <x:v>143</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2702,6 +2945,402 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
+  <x:dimension ref="A1:D45"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:4">
+      <x:c r="A1" s="1" t="s">
+        <x:v>160</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4">
+      <x:c r="B2" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C2" s="2" t="s">
+        <x:v>161</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4"/>
+    <x:row r="5" spans="1:4">
+      <x:c r="B5" s="1" t="s">
+        <x:v>162</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:4">
+      <x:c r="B6" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C6" s="2" t="s">
+        <x:v>163</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:4"/>
+    <x:row r="8" spans="1:4">
+      <x:c r="C8" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>164</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:4">
+      <x:c r="C9" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>165</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:4">
+      <x:c r="C10" s="3" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>166</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:4">
+      <x:c r="B12" s="1" t="s">
+        <x:v>146</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:4">
+      <x:c r="B13" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C13" s="2" t="s">
+        <x:v>167</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:4"/>
+    <x:row r="15" spans="1:4">
+      <x:c r="C15" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>168</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:4">
+      <x:c r="C16" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>165</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:4">
+      <x:c r="C17" s="3" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>169</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:4">
+      <x:c r="B19" s="1" t="s">
+        <x:v>170</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:4">
+      <x:c r="B20" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C20" s="2" t="s">
+        <x:v>171</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:4"/>
+    <x:row r="22" spans="1:4">
+      <x:c r="C22" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>172</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:4">
+      <x:c r="C23" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>165</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:4">
+      <x:c r="C24" s="3" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>169</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:4">
+      <x:c r="B26" s="1" t="s">
+        <x:v>162</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:4">
+      <x:c r="B27" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C27" s="2" t="s">
+        <x:v>173</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:4"/>
+    <x:row r="29" spans="1:4">
+      <x:c r="C29" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>164</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:4">
+      <x:c r="C30" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>174</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:4">
+      <x:c r="C31" s="3" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>166</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:4">
+      <x:c r="B33" s="1" t="s">
+        <x:v>146</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:4">
+      <x:c r="B34" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C34" s="2" t="s">
+        <x:v>175</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:4"/>
+    <x:row r="36" spans="1:4">
+      <x:c r="C36" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="s">
+        <x:v>168</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:4">
+      <x:c r="C37" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D37" s="0" t="s">
+        <x:v>176</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:4">
+      <x:c r="C38" s="3" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>177</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:4">
+      <x:c r="B40" s="1" t="s">
+        <x:v>170</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:4">
+      <x:c r="B41" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C41" s="2" t="s">
+        <x:v>178</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:4"/>
+    <x:row r="43" spans="1:4">
+      <x:c r="C43" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D43" s="0" t="s">
+        <x:v>172</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:4">
+      <x:c r="C44" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D44" s="0" t="s">
+        <x:v>176</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:4">
+      <x:c r="C45" s="3" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D45" s="0" t="s">
+        <x:v>177</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:D20"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:4">
+      <x:c r="A1" s="1" t="s">
+        <x:v>179</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4">
+      <x:c r="B2" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C2" s="2" t="s">
+        <x:v>180</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4"/>
+    <x:row r="5" spans="1:4">
+      <x:c r="B5" s="1" t="s">
+        <x:v>181</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:4">
+      <x:c r="B6" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C6" s="2" t="s">
+        <x:v>182</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:4"/>
+    <x:row r="8" spans="1:4">
+      <x:c r="C8" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>183</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:4">
+      <x:c r="C9" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>184</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:4">
+      <x:c r="C10" s="3" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>185</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:4">
+      <x:c r="B12" s="1" t="s">
+        <x:v>186</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:4">
+      <x:c r="B13" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C13" s="2" t="s">
+        <x:v>187</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:4"/>
+    <x:row r="15" spans="1:4">
+      <x:c r="C15" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>188</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:4">
+      <x:c r="C16" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>184</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:4">
+      <x:c r="C17" s="3" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>185</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:4">
+      <x:c r="C18" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>189</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:4">
+      <x:c r="C19" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>190</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:4">
+      <x:c r="C20" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>191</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
   <x:dimension ref="A1:D19"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
@@ -2710,7 +3349,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="1" t="s">
-        <x:v>151</x:v>
+        <x:v>192</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
@@ -2718,13 +3357,13 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>152</x:v>
+        <x:v>193</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4"/>
     <x:row r="5" spans="1:4">
       <x:c r="B5" s="1" t="s">
-        <x:v>153</x:v>
+        <x:v>194</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
@@ -2732,7 +3371,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>154</x:v>
+        <x:v>195</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4"/>
@@ -2741,7 +3380,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>155</x:v>
+        <x:v>196</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
@@ -2749,7 +3388,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>156</x:v>
+        <x:v>197</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
@@ -2757,7 +3396,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>157</x:v>
+        <x:v>198</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
@@ -2765,12 +3404,12 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>158</x:v>
+        <x:v>199</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
       <x:c r="B13" s="1" t="s">
-        <x:v>159</x:v>
+        <x:v>200</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4">
@@ -2778,7 +3417,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C14" s="2" t="s">
-        <x:v>160</x:v>
+        <x:v>201</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4"/>
@@ -2787,7 +3426,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>155</x:v>
+        <x:v>196</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4">
@@ -2795,7 +3434,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>156</x:v>
+        <x:v>197</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:4">
@@ -2803,7 +3442,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>157</x:v>
+        <x:v>198</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
@@ -2811,7 +3450,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>202</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>